<commit_message>
ajout du niveau suivant
</commit_message>
<xml_diff>
--- a/fizzbuzz.xlsx
+++ b/fizzbuzz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jydel\OneDrive\Desktop\FizzBuzz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1B0DE9-08D3-4E70-B52A-09153713E654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A9C4B2-3CD6-4B4C-B2BE-FB52423FEA10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{ABC71DB8-80FE-454F-B082-C51C83431DFA}"/>
   </bookViews>
@@ -40,7 +40,7 @@
     <t>nbre premier</t>
   </si>
   <si>
-    <t>quantité de nbre premier</t>
+    <t>quantité de nbre</t>
   </si>
 </sst>
 </file>
@@ -79,7 +79,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -543,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8694F71-8E0C-4B22-926B-201C15D2D012}">
-  <dimension ref="A1:L100"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -556,7 +556,7 @@
     <col min="9" max="9" width="10.90625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1">
         <v>1</v>
       </c>
@@ -564,21 +564,17 @@
         <v>1</v>
       </c>
       <c r="H1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I1" s="12">
         <f>+H1*G1</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J1">
-        <v>7</v>
-      </c>
-      <c r="L1">
-        <f>J1*G1</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>2</v>
       </c>
@@ -592,21 +588,17 @@
         <v>2</v>
       </c>
       <c r="H2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I2" s="12">
         <f t="shared" ref="I2:I9" si="0">+H2*G2</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J2">
-        <v>7</v>
-      </c>
-      <c r="L2">
-        <f t="shared" ref="L2:L14" si="1">J2*G2</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>3</v>
       </c>
@@ -620,21 +612,17 @@
         <v>3</v>
       </c>
       <c r="H3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I3" s="12">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J3">
-        <v>7</v>
-      </c>
-      <c r="L3">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>4</v>
       </c>
@@ -648,21 +636,17 @@
         <v>4</v>
       </c>
       <c r="H4">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I4" s="12">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="J4">
-        <v>7</v>
-      </c>
-      <c r="L4">
-        <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>5</v>
       </c>
@@ -676,21 +660,17 @@
         <v>5</v>
       </c>
       <c r="H5">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I5" s="12">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="J5">
-        <v>7</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>6</v>
       </c>
@@ -704,21 +684,17 @@
         <v>6</v>
       </c>
       <c r="H6">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I6" s="12">
         <f t="shared" si="0"/>
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="J6">
-        <v>7</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="1"/>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>7</v>
       </c>
@@ -732,25 +708,17 @@
         <v>7</v>
       </c>
       <c r="H7">
-        <v>11</v>
-      </c>
-      <c r="I7" s="13">
+        <v>7</v>
+      </c>
+      <c r="I7" s="12">
         <f t="shared" si="0"/>
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="J7">
-        <v>7</v>
-      </c>
-      <c r="K7">
-        <f t="shared" ref="K1:K31" si="2">+I7/J7</f>
-        <v>11</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="1"/>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>8</v>
       </c>
@@ -760,21 +728,17 @@
         <v>8</v>
       </c>
       <c r="H8">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I8" s="12">
         <f t="shared" si="0"/>
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="J8">
-        <v>7</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="1"/>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>9</v>
       </c>
@@ -788,21 +752,17 @@
         <v>9</v>
       </c>
       <c r="H9">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I9" s="12">
         <f t="shared" si="0"/>
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="J9">
-        <v>7</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="1"/>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>10</v>
       </c>
@@ -816,21 +776,17 @@
         <v>10</v>
       </c>
       <c r="H10">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I10" s="12">
-        <f t="shared" ref="I10:I14" si="3">+H10*G10</f>
-        <v>110</v>
+        <f t="shared" ref="I10:I14" si="1">+H10*G10</f>
+        <v>70</v>
       </c>
       <c r="J10">
-        <v>7</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>11</v>
       </c>
@@ -844,21 +800,21 @@
         <v>11</v>
       </c>
       <c r="H11">
-        <v>11</v>
-      </c>
-      <c r="I11" s="12">
-        <f t="shared" si="3"/>
-        <v>121</v>
-      </c>
-      <c r="J11">
-        <v>7</v>
-      </c>
-      <c r="L11">
+        <v>7</v>
+      </c>
+      <c r="I11" s="13">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="J11">
+        <v>11</v>
+      </c>
+      <c r="K11">
+        <f t="shared" ref="K7:K29" si="2">+I11/J11</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>12</v>
       </c>
@@ -872,21 +828,17 @@
         <v>12</v>
       </c>
       <c r="H12">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I12" s="12">
-        <f t="shared" si="3"/>
-        <v>132</v>
-      </c>
-      <c r="J12">
-        <v>7</v>
-      </c>
-      <c r="L12">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="J12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>13</v>
       </c>
@@ -896,21 +848,17 @@
         <v>13</v>
       </c>
       <c r="H13">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I13" s="12">
-        <f t="shared" si="3"/>
-        <v>143</v>
-      </c>
-      <c r="J13">
-        <v>7</v>
-      </c>
-      <c r="L13">
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="J13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>14</v>
       </c>
@@ -924,21 +872,17 @@
         <v>14</v>
       </c>
       <c r="H14">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I14" s="12">
-        <f t="shared" si="3"/>
-        <v>154</v>
+        <f>+H14*G14</f>
+        <v>98</v>
       </c>
       <c r="J14">
-        <v>7</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>15</v>
       </c>
@@ -952,21 +896,17 @@
         <v>15</v>
       </c>
       <c r="H15">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I15" s="12">
-        <f t="shared" ref="I15:I20" si="4">+H15*G15</f>
-        <v>165</v>
+        <f t="shared" ref="I15:I20" si="3">+H15*G15</f>
+        <v>105</v>
       </c>
       <c r="J15">
-        <v>7</v>
-      </c>
-      <c r="L15">
-        <f t="shared" ref="L15:L31" si="5">J15*G15</f>
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>16</v>
       </c>
@@ -980,21 +920,17 @@
         <v>16</v>
       </c>
       <c r="H16">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I16" s="12">
-        <f t="shared" si="4"/>
-        <v>176</v>
+        <f t="shared" si="3"/>
+        <v>112</v>
       </c>
       <c r="J16">
-        <v>7</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="5"/>
-        <v>112</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>17</v>
       </c>
@@ -1004,21 +940,17 @@
         <v>17</v>
       </c>
       <c r="H17">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I17" s="12">
-        <f t="shared" si="4"/>
-        <v>187</v>
+        <f t="shared" si="3"/>
+        <v>119</v>
       </c>
       <c r="J17">
-        <v>7</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="5"/>
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>18</v>
       </c>
@@ -1032,21 +964,17 @@
         <v>18</v>
       </c>
       <c r="H18">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I18" s="12">
-        <f t="shared" si="4"/>
-        <v>198</v>
+        <f t="shared" si="3"/>
+        <v>126</v>
       </c>
       <c r="J18">
-        <v>7</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="5"/>
-        <v>126</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>19</v>
       </c>
@@ -1060,21 +988,17 @@
         <v>19</v>
       </c>
       <c r="H19">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I19" s="12">
-        <f t="shared" si="4"/>
-        <v>209</v>
+        <f t="shared" si="3"/>
+        <v>133</v>
       </c>
       <c r="J19">
-        <v>7</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="5"/>
-        <v>133</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>20</v>
       </c>
@@ -1084,21 +1008,17 @@
         <v>20</v>
       </c>
       <c r="H20">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I20" s="12">
-        <f t="shared" si="4"/>
-        <v>220</v>
+        <f t="shared" si="3"/>
+        <v>140</v>
       </c>
       <c r="J20">
-        <v>7</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="5"/>
-        <v>140</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>21</v>
       </c>
@@ -1112,17 +1032,13 @@
         <v>21</v>
       </c>
       <c r="H21">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="J21">
-        <v>7</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="5"/>
-        <v>147</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>22</v>
       </c>
@@ -1130,17 +1046,13 @@
         <v>22</v>
       </c>
       <c r="H22">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="J22">
-        <v>7</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="5"/>
-        <v>154</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>23</v>
       </c>
@@ -1148,17 +1060,13 @@
         <v>23</v>
       </c>
       <c r="H23">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="J23">
-        <v>7</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="5"/>
-        <v>161</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>24</v>
       </c>
@@ -1166,17 +1074,13 @@
         <v>24</v>
       </c>
       <c r="H24">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="J24">
-        <v>7</v>
-      </c>
-      <c r="L24">
-        <f t="shared" si="5"/>
-        <v>168</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>25</v>
       </c>
@@ -1184,17 +1088,13 @@
         <v>25</v>
       </c>
       <c r="H25">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="J25">
-        <v>7</v>
-      </c>
-      <c r="L25">
-        <f t="shared" si="5"/>
-        <v>175</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>26</v>
       </c>
@@ -1202,17 +1102,13 @@
         <v>26</v>
       </c>
       <c r="H26">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="J26">
-        <v>7</v>
-      </c>
-      <c r="L26">
-        <f t="shared" si="5"/>
-        <v>182</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>27</v>
       </c>
@@ -1220,17 +1116,13 @@
         <v>27</v>
       </c>
       <c r="H27">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="J27">
-        <v>7</v>
-      </c>
-      <c r="L27">
-        <f t="shared" si="5"/>
-        <v>189</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>28</v>
       </c>
@@ -1238,17 +1130,13 @@
         <v>28</v>
       </c>
       <c r="H28">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="J28">
-        <v>7</v>
-      </c>
-      <c r="L28">
-        <f t="shared" si="5"/>
-        <v>196</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>29</v>
       </c>
@@ -1256,17 +1144,13 @@
         <v>29</v>
       </c>
       <c r="H29">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="J29">
-        <v>7</v>
-      </c>
-      <c r="L29">
-        <f t="shared" si="5"/>
-        <v>203</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>30</v>
       </c>
@@ -1274,17 +1158,13 @@
         <v>30</v>
       </c>
       <c r="H30">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="J30">
-        <v>7</v>
-      </c>
-      <c r="L30">
-        <f t="shared" si="5"/>
-        <v>210</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>31</v>
       </c>
@@ -1292,17 +1172,13 @@
         <v>31</v>
       </c>
       <c r="H31">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="J31">
-        <v>7</v>
-      </c>
-      <c r="L31">
-        <f t="shared" si="5"/>
-        <v>217</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
fizz buee et fizzbuzz sous forme matricielle
</commit_message>
<xml_diff>
--- a/fizzbuzz.xlsx
+++ b/fizzbuzz.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jydel\OneDrive\Desktop\FizzBuzz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A9C4B2-3CD6-4B4C-B2BE-FB52423FEA10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2651E382-02E7-4E86-80B2-070AD76B2C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{ABC71DB8-80FE-454F-B082-C51C83431DFA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{ABC71DB8-80FE-454F-B082-C51C83431DFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="fizz et buzz" sheetId="3" r:id="rId2"/>
+    <sheet name="fizzbuzz" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,19 +37,61 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="16">
   <si>
     <t>nbre premier</t>
   </si>
   <si>
     <t>quantité de nbre</t>
   </si>
+  <si>
+    <t xml:space="preserve">              </t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>M4</t>
+  </si>
+  <si>
+    <t>M5</t>
+  </si>
+  <si>
+    <t>M6</t>
+  </si>
+  <si>
+    <t>M7</t>
+  </si>
+  <si>
+    <t>M8</t>
+  </si>
+  <si>
+    <t>M9</t>
+  </si>
+  <si>
+    <t>M10</t>
+  </si>
+  <si>
+    <t>couple</t>
+  </si>
+  <si>
+    <t>nbre fizzbuzz</t>
+  </si>
+  <si>
+    <t>NBRE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,6 +102,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -84,7 +136,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -210,11 +262,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -229,6 +296,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,15 +646,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8694F71-8E0C-4B22-926B-201C15D2D012}">
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="C3:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="14.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.90625" style="12"/>
+    <col min="9" max="9" width="10.81640625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -656,6 +757,9 @@
       <c r="D5" s="6">
         <v>20</v>
       </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
       <c r="G5">
         <v>5</v>
       </c>
@@ -748,6 +852,13 @@
       <c r="D9" s="6">
         <v>17</v>
       </c>
+      <c r="E9">
+        <f>D9/10</f>
+        <v>1.7</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
       <c r="G9">
         <v>9</v>
       </c>
@@ -772,6 +883,13 @@
       <c r="D10" s="6">
         <v>11</v>
       </c>
+      <c r="E10">
+        <f t="shared" ref="E10:E21" si="1">D10/10</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
       <c r="G10">
         <v>10</v>
       </c>
@@ -779,7 +897,7 @@
         <v>7</v>
       </c>
       <c r="I10" s="12">
-        <f t="shared" ref="I10:I14" si="1">+H10*G10</f>
+        <f t="shared" ref="I10:I13" si="2">+H10*G10</f>
         <v>70</v>
       </c>
       <c r="J10">
@@ -796,6 +914,13 @@
       <c r="D11" s="6">
         <v>8</v>
       </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
       <c r="G11">
         <v>11</v>
       </c>
@@ -803,14 +928,14 @@
         <v>7</v>
       </c>
       <c r="I11" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>77</v>
       </c>
       <c r="J11">
         <v>11</v>
       </c>
       <c r="K11">
-        <f t="shared" ref="K7:K29" si="2">+I11/J11</f>
+        <f t="shared" ref="K11" si="3">+I11/J11</f>
         <v>7</v>
       </c>
     </row>
@@ -824,6 +949,13 @@
       <c r="D12" s="6">
         <v>5</v>
       </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
       <c r="G12">
         <v>12</v>
       </c>
@@ -831,7 +963,7 @@
         <v>7</v>
       </c>
       <c r="I12" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>84</v>
       </c>
       <c r="J12">
@@ -844,6 +976,10 @@
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="G13">
         <v>13</v>
       </c>
@@ -851,7 +987,7 @@
         <v>7</v>
       </c>
       <c r="I13" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>91</v>
       </c>
       <c r="J13">
@@ -868,6 +1004,13 @@
       <c r="D14" s="6">
         <v>7</v>
       </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>0.7</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
       <c r="G14">
         <v>14</v>
       </c>
@@ -892,6 +1035,13 @@
       <c r="D15" s="6">
         <v>5</v>
       </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
       <c r="G15">
         <v>15</v>
       </c>
@@ -899,7 +1049,7 @@
         <v>7</v>
       </c>
       <c r="I15" s="12">
-        <f t="shared" ref="I15:I20" si="3">+H15*G15</f>
+        <f t="shared" ref="I15:I20" si="4">+H15*G15</f>
         <v>105</v>
       </c>
       <c r="J15">
@@ -916,6 +1066,13 @@
       <c r="D16" s="6">
         <v>4</v>
       </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
       <c r="G16">
         <v>16</v>
       </c>
@@ -923,7 +1080,7 @@
         <v>7</v>
       </c>
       <c r="I16" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>112</v>
       </c>
       <c r="J16">
@@ -936,6 +1093,10 @@
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="8"/>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="G17">
         <v>17</v>
       </c>
@@ -943,7 +1104,7 @@
         <v>7</v>
       </c>
       <c r="I17" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>119</v>
       </c>
       <c r="J17">
@@ -960,6 +1121,13 @@
       <c r="D18" s="6">
         <v>3</v>
       </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>0.3</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
       <c r="G18">
         <v>18</v>
       </c>
@@ -967,7 +1135,7 @@
         <v>7</v>
       </c>
       <c r="I18" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>126</v>
       </c>
       <c r="J18">
@@ -984,6 +1152,13 @@
       <c r="D19" s="6">
         <v>2</v>
       </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
       <c r="G19">
         <v>19</v>
       </c>
@@ -991,7 +1166,7 @@
         <v>7</v>
       </c>
       <c r="I19" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>133</v>
       </c>
       <c r="J19">
@@ -1002,8 +1177,12 @@
       <c r="A20">
         <v>20</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="8"/>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="G20">
         <v>20</v>
       </c>
@@ -1011,7 +1190,7 @@
         <v>7</v>
       </c>
       <c r="I20" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>140</v>
       </c>
       <c r="J20">
@@ -1027,6 +1206,13 @@
       </c>
       <c r="D21" s="10">
         <v>2</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
       </c>
       <c r="G21">
         <v>21</v>
@@ -1527,4 +1713,1288 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB2EF8FE-7976-455F-A7A2-652D6E5C5BD6}">
+  <dimension ref="A1:N28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="3">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" s="5">
+        <v>3</v>
+      </c>
+      <c r="B2" s="6">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" s="5">
+        <v>5</v>
+      </c>
+      <c r="B3" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" s="5">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" s="5">
+        <v>11</v>
+      </c>
+      <c r="B5" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="N8" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" s="5">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B9" s="6">
+        <v>17</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="14">
+        <v>2</v>
+      </c>
+      <c r="E9" s="16">
+        <v>5</v>
+      </c>
+      <c r="F9" s="16">
+        <v>10</v>
+      </c>
+      <c r="G9" s="16">
+        <v>15</v>
+      </c>
+      <c r="H9" s="16">
+        <v>20</v>
+      </c>
+      <c r="I9" s="16">
+        <v>25</v>
+      </c>
+      <c r="J9" s="16">
+        <v>30</v>
+      </c>
+      <c r="K9" s="16">
+        <v>35</v>
+      </c>
+      <c r="L9" s="16">
+        <v>40</v>
+      </c>
+      <c r="M9" s="16">
+        <v>45</v>
+      </c>
+      <c r="N9" s="16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="B10" s="6">
+        <v>11</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="14">
+        <v>3</v>
+      </c>
+      <c r="E10" s="16">
+        <v>5</v>
+      </c>
+      <c r="F10" s="16">
+        <v>8</v>
+      </c>
+      <c r="G10" s="16">
+        <v>10</v>
+      </c>
+      <c r="H10" s="16">
+        <v>13</v>
+      </c>
+      <c r="I10" s="16">
+        <v>16</v>
+      </c>
+      <c r="J10" s="16">
+        <v>18</v>
+      </c>
+      <c r="K10" s="16">
+        <v>20</v>
+      </c>
+      <c r="L10" s="16">
+        <v>23</v>
+      </c>
+      <c r="M10" s="16">
+        <v>27</v>
+      </c>
+      <c r="N10" s="16">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" s="5">
+        <v>2.7</v>
+      </c>
+      <c r="B11" s="6">
+        <v>8</v>
+      </c>
+      <c r="D11" s="15">
+        <v>5</v>
+      </c>
+      <c r="E11" s="16">
+        <v>2</v>
+      </c>
+      <c r="F11" s="16">
+        <v>4</v>
+      </c>
+      <c r="G11" s="16">
+        <v>6</v>
+      </c>
+      <c r="H11" s="16">
+        <v>8</v>
+      </c>
+      <c r="I11" s="16">
+        <v>10</v>
+      </c>
+      <c r="J11" s="16">
+        <v>12</v>
+      </c>
+      <c r="K11" s="16">
+        <v>14</v>
+      </c>
+      <c r="L11" s="16">
+        <v>16</v>
+      </c>
+      <c r="M11" s="16">
+        <v>18</v>
+      </c>
+      <c r="N11" s="16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" s="5">
+        <v>2.11</v>
+      </c>
+      <c r="B12" s="6">
+        <v>5</v>
+      </c>
+      <c r="D12" s="16">
+        <v>7</v>
+      </c>
+      <c r="E12" s="16">
+        <v>2</v>
+      </c>
+      <c r="F12" s="16">
+        <v>3</v>
+      </c>
+      <c r="G12" s="16">
+        <v>4</v>
+      </c>
+      <c r="H12" s="16">
+        <v>5</v>
+      </c>
+      <c r="I12" s="16">
+        <v>7</v>
+      </c>
+      <c r="J12" s="16">
+        <v>9</v>
+      </c>
+      <c r="K12" s="16">
+        <v>11</v>
+      </c>
+      <c r="L12" s="16">
+        <v>12</v>
+      </c>
+      <c r="M12" s="16">
+        <v>13</v>
+      </c>
+      <c r="N12" s="16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="D13" s="16">
+        <v>11</v>
+      </c>
+      <c r="E13" s="16">
+        <v>2</v>
+      </c>
+      <c r="F13" s="16">
+        <v>2</v>
+      </c>
+      <c r="G13" s="16">
+        <v>3</v>
+      </c>
+      <c r="H13" s="16">
+        <v>4</v>
+      </c>
+      <c r="I13" s="16">
+        <v>5</v>
+      </c>
+      <c r="J13" s="16">
+        <v>6</v>
+      </c>
+      <c r="K13" s="16">
+        <v>7</v>
+      </c>
+      <c r="L13" s="16">
+        <v>8</v>
+      </c>
+      <c r="M13" s="16">
+        <v>9</v>
+      </c>
+      <c r="N13" s="16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="B14" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" s="5">
+        <v>3.7</v>
+      </c>
+      <c r="B15" s="6">
+        <v>5</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="L15" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M15" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="N15" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16" s="5">
+        <v>3.11</v>
+      </c>
+      <c r="B16" s="6">
+        <v>4</v>
+      </c>
+      <c r="D16" s="19">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E16" s="16">
+        <v>2</v>
+      </c>
+      <c r="F16" s="16">
+        <v>4</v>
+      </c>
+      <c r="G16" s="16">
+        <v>6</v>
+      </c>
+      <c r="H16" s="16">
+        <v>8</v>
+      </c>
+      <c r="I16" s="16">
+        <v>10</v>
+      </c>
+      <c r="J16" s="16">
+        <v>12</v>
+      </c>
+      <c r="K16" s="16">
+        <v>14</v>
+      </c>
+      <c r="L16" s="16">
+        <v>16</v>
+      </c>
+      <c r="M16" s="16">
+        <v>17</v>
+      </c>
+      <c r="N16" s="16">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="D17" s="19">
+        <v>2.5</v>
+      </c>
+      <c r="E17" s="16">
+        <v>1</v>
+      </c>
+      <c r="F17" s="16">
+        <v>2</v>
+      </c>
+      <c r="G17" s="16">
+        <v>3</v>
+      </c>
+      <c r="H17" s="17">
+        <v>4</v>
+      </c>
+      <c r="I17" s="16">
+        <v>5</v>
+      </c>
+      <c r="J17" s="16">
+        <v>6</v>
+      </c>
+      <c r="K17" s="16">
+        <v>7</v>
+      </c>
+      <c r="L17" s="16">
+        <v>8</v>
+      </c>
+      <c r="M17" s="16">
+        <v>9</v>
+      </c>
+      <c r="N17" s="16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" s="5">
+        <v>5.7</v>
+      </c>
+      <c r="B18" s="6">
+        <v>3</v>
+      </c>
+      <c r="D18" s="19">
+        <v>2.7</v>
+      </c>
+      <c r="E18" s="16">
+        <v>1</v>
+      </c>
+      <c r="F18" s="16">
+        <v>2</v>
+      </c>
+      <c r="G18" s="16">
+        <v>2</v>
+      </c>
+      <c r="H18" s="17">
+        <v>3</v>
+      </c>
+      <c r="I18" s="16">
+        <v>4</v>
+      </c>
+      <c r="J18" s="16">
+        <v>4</v>
+      </c>
+      <c r="K18" s="16">
+        <v>5</v>
+      </c>
+      <c r="L18" s="16">
+        <v>6</v>
+      </c>
+      <c r="M18" s="16">
+        <v>7</v>
+      </c>
+      <c r="N18" s="16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" s="5">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="B19" s="6">
+        <v>2</v>
+      </c>
+      <c r="D19" s="19">
+        <v>2.11</v>
+      </c>
+      <c r="E19" s="16">
+        <v>1</v>
+      </c>
+      <c r="F19" s="16">
+        <v>1</v>
+      </c>
+      <c r="G19" s="16">
+        <v>2</v>
+      </c>
+      <c r="H19" s="17">
+        <v>2</v>
+      </c>
+      <c r="I19" s="16">
+        <v>3</v>
+      </c>
+      <c r="J19" s="16">
+        <v>3</v>
+      </c>
+      <c r="K19" s="16">
+        <v>4</v>
+      </c>
+      <c r="L19" s="16">
+        <v>4</v>
+      </c>
+      <c r="M19" s="16">
+        <v>5</v>
+      </c>
+      <c r="N19" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
+    </row>
+    <row r="21" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="9">
+        <v>7.11</v>
+      </c>
+      <c r="B21" s="10">
+        <v>2</v>
+      </c>
+      <c r="D21" s="19">
+        <v>3.5</v>
+      </c>
+      <c r="E21" s="16">
+        <v>1</v>
+      </c>
+      <c r="F21" s="16">
+        <v>1</v>
+      </c>
+      <c r="G21" s="16">
+        <v>2</v>
+      </c>
+      <c r="H21" s="17">
+        <v>3</v>
+      </c>
+      <c r="I21" s="16">
+        <v>3</v>
+      </c>
+      <c r="J21" s="16">
+        <v>4</v>
+      </c>
+      <c r="K21" s="16">
+        <v>5</v>
+      </c>
+      <c r="L21" s="16">
+        <v>5</v>
+      </c>
+      <c r="M21" s="16">
+        <v>6</v>
+      </c>
+      <c r="N21" s="16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="D22" s="19">
+        <v>3.7</v>
+      </c>
+      <c r="E22" s="16">
+        <v>1</v>
+      </c>
+      <c r="F22" s="16">
+        <v>1</v>
+      </c>
+      <c r="G22" s="16">
+        <v>2</v>
+      </c>
+      <c r="H22" s="17">
+        <v>2</v>
+      </c>
+      <c r="I22" s="16">
+        <v>2</v>
+      </c>
+      <c r="J22" s="16">
+        <v>3</v>
+      </c>
+      <c r="K22" s="16">
+        <v>3</v>
+      </c>
+      <c r="L22" s="16">
+        <v>4</v>
+      </c>
+      <c r="M22" s="16">
+        <v>4</v>
+      </c>
+      <c r="N22" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="D23" s="19">
+        <v>3.11</v>
+      </c>
+      <c r="E23" s="16">
+        <v>1</v>
+      </c>
+      <c r="F23" s="16">
+        <v>1</v>
+      </c>
+      <c r="G23" s="16">
+        <v>2</v>
+      </c>
+      <c r="H23" s="17">
+        <v>2</v>
+      </c>
+      <c r="I23" s="16">
+        <v>2</v>
+      </c>
+      <c r="J23" s="16">
+        <v>3</v>
+      </c>
+      <c r="K23" s="16">
+        <v>3</v>
+      </c>
+      <c r="L23" s="16">
+        <v>3</v>
+      </c>
+      <c r="M23" s="16">
+        <v>4</v>
+      </c>
+      <c r="N23" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="21"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="D25" s="19">
+        <v>5.7</v>
+      </c>
+      <c r="E25" s="16">
+        <v>1</v>
+      </c>
+      <c r="F25" s="16">
+        <v>1</v>
+      </c>
+      <c r="G25" s="16">
+        <v>1</v>
+      </c>
+      <c r="H25" s="17">
+        <v>1</v>
+      </c>
+      <c r="I25" s="16">
+        <v>1</v>
+      </c>
+      <c r="J25" s="16">
+        <v>2</v>
+      </c>
+      <c r="K25" s="16">
+        <v>2</v>
+      </c>
+      <c r="L25" s="16">
+        <v>2</v>
+      </c>
+      <c r="M25" s="16">
+        <v>3</v>
+      </c>
+      <c r="N25" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="D26" s="19">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="E26" s="16">
+        <v>1</v>
+      </c>
+      <c r="F26" s="16">
+        <v>1</v>
+      </c>
+      <c r="G26" s="16">
+        <v>1</v>
+      </c>
+      <c r="H26" s="17">
+        <v>1</v>
+      </c>
+      <c r="I26" s="16">
+        <v>1</v>
+      </c>
+      <c r="J26" s="16">
+        <v>1</v>
+      </c>
+      <c r="K26" s="16">
+        <v>2</v>
+      </c>
+      <c r="L26" s="16">
+        <v>2</v>
+      </c>
+      <c r="M26" s="16">
+        <v>2</v>
+      </c>
+      <c r="N26" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="21"/>
+    </row>
+    <row r="28" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D28" s="23">
+        <v>7.11</v>
+      </c>
+      <c r="E28" s="16">
+        <v>1</v>
+      </c>
+      <c r="F28" s="16">
+        <v>1</v>
+      </c>
+      <c r="G28" s="16">
+        <v>1</v>
+      </c>
+      <c r="H28" s="17">
+        <v>1</v>
+      </c>
+      <c r="I28" s="16">
+        <v>1</v>
+      </c>
+      <c r="J28" s="16">
+        <v>1</v>
+      </c>
+      <c r="K28" s="16">
+        <v>2</v>
+      </c>
+      <c r="L28" s="16">
+        <v>2</v>
+      </c>
+      <c r="M28" s="16">
+        <v>2</v>
+      </c>
+      <c r="N28" s="16">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{827DEE83-DD30-43E1-B52F-7963A59877FB}">
+  <dimension ref="A1:M15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:M15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="G1" s="12"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="19">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B3" s="20">
+        <v>17</v>
+      </c>
+      <c r="C3">
+        <f>B3/10</f>
+        <v>1.7</v>
+      </c>
+      <c r="D3" s="16">
+        <v>2</v>
+      </c>
+      <c r="E3" s="16">
+        <v>4</v>
+      </c>
+      <c r="F3" s="16">
+        <v>6</v>
+      </c>
+      <c r="G3" s="16">
+        <v>8</v>
+      </c>
+      <c r="H3" s="16">
+        <v>10</v>
+      </c>
+      <c r="I3" s="16">
+        <v>12</v>
+      </c>
+      <c r="J3" s="16">
+        <v>14</v>
+      </c>
+      <c r="K3" s="16">
+        <v>16</v>
+      </c>
+      <c r="L3" s="16">
+        <v>17</v>
+      </c>
+      <c r="M3" s="16">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" s="19">
+        <v>2.5</v>
+      </c>
+      <c r="B4" s="20">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <f>B4/10</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D4" s="16">
+        <v>1</v>
+      </c>
+      <c r="E4" s="16">
+        <v>2</v>
+      </c>
+      <c r="F4" s="16">
+        <v>3</v>
+      </c>
+      <c r="G4" s="17">
+        <v>4</v>
+      </c>
+      <c r="H4" s="16">
+        <v>5</v>
+      </c>
+      <c r="I4" s="16">
+        <v>6</v>
+      </c>
+      <c r="J4" s="16">
+        <v>7</v>
+      </c>
+      <c r="K4" s="16">
+        <v>8</v>
+      </c>
+      <c r="L4" s="16">
+        <v>9</v>
+      </c>
+      <c r="M4" s="16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" s="19">
+        <v>2.7</v>
+      </c>
+      <c r="B5" s="20">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <f>B5/10</f>
+        <v>0.8</v>
+      </c>
+      <c r="D5" s="16">
+        <v>1</v>
+      </c>
+      <c r="E5" s="16">
+        <v>2</v>
+      </c>
+      <c r="F5" s="16">
+        <v>2</v>
+      </c>
+      <c r="G5" s="17">
+        <v>3</v>
+      </c>
+      <c r="H5" s="16">
+        <v>4</v>
+      </c>
+      <c r="I5" s="16">
+        <v>4</v>
+      </c>
+      <c r="J5" s="16">
+        <v>5</v>
+      </c>
+      <c r="K5" s="16">
+        <v>6</v>
+      </c>
+      <c r="L5" s="16">
+        <v>7</v>
+      </c>
+      <c r="M5" s="16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="19">
+        <v>2.11</v>
+      </c>
+      <c r="B6" s="20">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <f>B6/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="16">
+        <v>1</v>
+      </c>
+      <c r="E6" s="16">
+        <v>1</v>
+      </c>
+      <c r="F6" s="16">
+        <v>2</v>
+      </c>
+      <c r="G6" s="17">
+        <v>2</v>
+      </c>
+      <c r="H6" s="16">
+        <v>3</v>
+      </c>
+      <c r="I6" s="16">
+        <v>3</v>
+      </c>
+      <c r="J6" s="16">
+        <v>4</v>
+      </c>
+      <c r="K6" s="16">
+        <v>4</v>
+      </c>
+      <c r="L6" s="16">
+        <v>5</v>
+      </c>
+      <c r="M6" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="21"/>
+      <c r="B7" s="22"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="19">
+        <v>3.5</v>
+      </c>
+      <c r="B8" s="20">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <f>B8/10</f>
+        <v>0.7</v>
+      </c>
+      <c r="D8" s="16">
+        <v>1</v>
+      </c>
+      <c r="E8" s="16">
+        <v>1</v>
+      </c>
+      <c r="F8" s="16">
+        <v>2</v>
+      </c>
+      <c r="G8" s="17">
+        <v>3</v>
+      </c>
+      <c r="H8" s="16">
+        <v>3</v>
+      </c>
+      <c r="I8" s="16">
+        <v>4</v>
+      </c>
+      <c r="J8" s="16">
+        <v>5</v>
+      </c>
+      <c r="K8" s="16">
+        <v>5</v>
+      </c>
+      <c r="L8" s="16">
+        <v>6</v>
+      </c>
+      <c r="M8" s="16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="19">
+        <v>3.7</v>
+      </c>
+      <c r="B9" s="20">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <f>B9/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="16">
+        <v>1</v>
+      </c>
+      <c r="E9" s="16">
+        <v>1</v>
+      </c>
+      <c r="F9" s="16">
+        <v>2</v>
+      </c>
+      <c r="G9" s="17">
+        <v>2</v>
+      </c>
+      <c r="H9" s="16">
+        <v>2</v>
+      </c>
+      <c r="I9" s="16">
+        <v>3</v>
+      </c>
+      <c r="J9" s="16">
+        <v>3</v>
+      </c>
+      <c r="K9" s="16">
+        <v>4</v>
+      </c>
+      <c r="L9" s="16">
+        <v>4</v>
+      </c>
+      <c r="M9" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="19">
+        <v>3.11</v>
+      </c>
+      <c r="B10" s="20">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <f>B10/10</f>
+        <v>0.4</v>
+      </c>
+      <c r="D10" s="16">
+        <v>1</v>
+      </c>
+      <c r="E10" s="16">
+        <v>1</v>
+      </c>
+      <c r="F10" s="16">
+        <v>2</v>
+      </c>
+      <c r="G10" s="17">
+        <v>2</v>
+      </c>
+      <c r="H10" s="16">
+        <v>2</v>
+      </c>
+      <c r="I10" s="16">
+        <v>3</v>
+      </c>
+      <c r="J10" s="16">
+        <v>3</v>
+      </c>
+      <c r="K10" s="16">
+        <v>3</v>
+      </c>
+      <c r="L10" s="16">
+        <v>4</v>
+      </c>
+      <c r="M10" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" s="21"/>
+      <c r="B11" s="22"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" s="19">
+        <v>5.7</v>
+      </c>
+      <c r="B12" s="20">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <f>B12/10</f>
+        <v>0.3</v>
+      </c>
+      <c r="D12" s="16">
+        <v>0</v>
+      </c>
+      <c r="E12" s="16">
+        <v>0</v>
+      </c>
+      <c r="F12" s="16">
+        <v>1</v>
+      </c>
+      <c r="G12" s="17">
+        <v>1</v>
+      </c>
+      <c r="H12" s="16">
+        <v>1</v>
+      </c>
+      <c r="I12" s="16">
+        <v>2</v>
+      </c>
+      <c r="J12" s="16">
+        <v>2</v>
+      </c>
+      <c r="K12" s="16">
+        <v>2</v>
+      </c>
+      <c r="L12" s="16">
+        <v>3</v>
+      </c>
+      <c r="M12" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" s="19">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="B13" s="20">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <f>B13/10</f>
+        <v>0.2</v>
+      </c>
+      <c r="D13" s="16">
+        <v>0</v>
+      </c>
+      <c r="E13" s="16">
+        <v>0</v>
+      </c>
+      <c r="F13" s="16">
+        <v>1</v>
+      </c>
+      <c r="G13" s="17">
+        <v>1</v>
+      </c>
+      <c r="H13" s="16">
+        <v>1</v>
+      </c>
+      <c r="I13" s="16">
+        <v>1</v>
+      </c>
+      <c r="J13" s="16">
+        <v>2</v>
+      </c>
+      <c r="K13" s="16">
+        <v>2</v>
+      </c>
+      <c r="L13" s="16">
+        <v>2</v>
+      </c>
+      <c r="M13" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+    </row>
+    <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="23">
+        <v>7.11</v>
+      </c>
+      <c r="B15" s="24">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <f>B15/10</f>
+        <v>0.2</v>
+      </c>
+      <c r="D15" s="16">
+        <v>0</v>
+      </c>
+      <c r="E15" s="16">
+        <v>0</v>
+      </c>
+      <c r="F15" s="16">
+        <v>1</v>
+      </c>
+      <c r="G15" s="17">
+        <v>1</v>
+      </c>
+      <c r="H15" s="16">
+        <v>1</v>
+      </c>
+      <c r="I15" s="16">
+        <v>1</v>
+      </c>
+      <c r="J15" s="16">
+        <v>2</v>
+      </c>
+      <c r="K15" s="16">
+        <v>2</v>
+      </c>
+      <c r="L15" s="16">
+        <v>2</v>
+      </c>
+      <c r="M15" s="16">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
passage d monde en monde OK
</commit_message>
<xml_diff>
--- a/fizzbuzz.xlsx
+++ b/fizzbuzz.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jydel\OneDrive\Desktop\FizzBuzz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2651E382-02E7-4E86-80B2-070AD76B2C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A85EADF-6EF7-45A6-82C7-48868DEEEE78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{ABC71DB8-80FE-454F-B082-C51C83431DFA}"/>
+    <workbookView xWindow="7890" yWindow="1005" windowWidth="12615" windowHeight="7200" xr2:uid="{ABC71DB8-80FE-454F-B082-C51C83431DFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +114,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -281,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -330,6 +336,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -644,20 +653,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8694F71-8E0C-4B22-926B-201C15D2D012}">
-  <dimension ref="A1:K100"/>
+  <dimension ref="A1:L100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="C3:D21"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.81640625" style="12"/>
+    <col min="3" max="3" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -675,7 +684,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2</v>
       </c>
@@ -699,7 +708,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -723,7 +732,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -747,7 +756,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -774,7 +783,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -797,8 +806,9 @@
       <c r="J6">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L6" s="26"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -822,7 +832,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -842,7 +852,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -873,7 +883,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -904,7 +914,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
@@ -939,7 +949,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
@@ -970,7 +980,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
@@ -994,7 +1004,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
@@ -1025,7 +1035,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
@@ -1056,7 +1066,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>
@@ -1087,7 +1097,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
@@ -1111,7 +1121,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18</v>
       </c>
@@ -1142,7 +1152,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
@@ -1173,7 +1183,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20</v>
       </c>
@@ -1197,7 +1207,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>21</v>
       </c>
@@ -1224,7 +1234,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>22</v>
       </c>
@@ -1238,7 +1248,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>23</v>
       </c>
@@ -1252,7 +1262,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>24</v>
       </c>
@@ -1266,7 +1276,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>25</v>
       </c>
@@ -1280,7 +1290,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>26</v>
       </c>
@@ -1294,7 +1304,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>27</v>
       </c>
@@ -1308,7 +1318,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>28</v>
       </c>
@@ -1322,7 +1332,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>29</v>
       </c>
@@ -1336,7 +1346,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>30</v>
       </c>
@@ -1350,7 +1360,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>31</v>
       </c>
@@ -1364,347 +1374,347 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>65</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>66</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>71</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>72</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>78</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>79</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>80</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>82</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>83</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>84</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>86</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>88</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>89</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>91</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>92</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>93</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>94</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>95</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>96</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>97</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>98</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>99</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>100</v>
       </c>
@@ -1719,13 +1729,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB2EF8FE-7976-455F-A7A2-652D6E5C5BD6}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3">
         <v>2</v>
       </c>
@@ -1733,7 +1743,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>3</v>
       </c>
@@ -1741,7 +1751,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>5</v>
       </c>
@@ -1749,7 +1759,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>7</v>
       </c>
@@ -1757,20 +1767,20 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>11</v>
       </c>
       <c r="B5" s="6">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="8"/>
       <c r="C8" s="1"/>
@@ -1808,7 +1818,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>2.2999999999999998</v>
       </c>
@@ -1850,7 +1860,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>2.5</v>
       </c>
@@ -1892,7 +1902,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>2.7</v>
       </c>
@@ -1933,7 +1943,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>2.11</v>
       </c>
@@ -1974,7 +1984,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="D13" s="16">
@@ -2011,7 +2021,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>3.5</v>
       </c>
@@ -2019,7 +2029,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>3.7</v>
       </c>
@@ -2057,7 +2067,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>3.11</v>
       </c>
@@ -2098,7 +2108,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="D17" s="19">
@@ -2135,7 +2145,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>5.7</v>
       </c>
@@ -2176,7 +2186,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>5.1100000000000003</v>
       </c>
@@ -2217,7 +2227,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="D20" s="21"/>
@@ -2232,7 +2242,7 @@
       <c r="M20" s="21"/>
       <c r="N20" s="21"/>
     </row>
-    <row r="21" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9">
         <v>7.11</v>
       </c>
@@ -2273,7 +2283,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D22" s="19">
         <v>3.7</v>
       </c>
@@ -2308,7 +2318,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D23" s="19">
         <v>3.11</v>
       </c>
@@ -2343,7 +2353,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
       <c r="F24" s="21"/>
@@ -2356,7 +2366,7 @@
       <c r="M24" s="21"/>
       <c r="N24" s="21"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D25" s="19">
         <v>5.7</v>
       </c>
@@ -2391,7 +2401,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D26" s="19">
         <v>5.1100000000000003</v>
       </c>
@@ -2426,7 +2436,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D27" s="21"/>
       <c r="E27" s="21"/>
       <c r="F27" s="21"/>
@@ -2439,7 +2449,7 @@
       <c r="M27" s="21"/>
       <c r="N27" s="21"/>
     </row>
-    <row r="28" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D28" s="23">
         <v>7.11</v>
       </c>
@@ -2487,14 +2497,14 @@
       <selection activeCell="C2" sqref="C2:M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="G1" s="12"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>13</v>
       </c>
@@ -2532,7 +2542,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="19">
         <v>2.2999999999999998</v>
       </c>
@@ -2574,7 +2584,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="19">
         <v>2.5</v>
       </c>
@@ -2616,7 +2626,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
         <v>2.7</v>
       </c>
@@ -2658,7 +2668,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
         <v>2.11</v>
       </c>
@@ -2700,7 +2710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
       <c r="B7" s="22"/>
       <c r="D7" s="21"/>
@@ -2714,7 +2724,7 @@
       <c r="L7" s="21"/>
       <c r="M7" s="21"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>3.5</v>
       </c>
@@ -2756,7 +2766,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
         <v>3.7</v>
       </c>
@@ -2798,7 +2808,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
         <v>3.11</v>
       </c>
@@ -2840,7 +2850,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
       <c r="B11" s="22"/>
       <c r="D11" s="21"/>
@@ -2854,7 +2864,7 @@
       <c r="L11" s="21"/>
       <c r="M11" s="21"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
         <v>5.7</v>
       </c>
@@ -2896,7 +2906,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
         <v>5.1100000000000003</v>
       </c>
@@ -2938,7 +2948,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="21"/>
       <c r="D14" s="21"/>
@@ -2952,7 +2962,7 @@
       <c r="L14" s="21"/>
       <c r="M14" s="21"/>
     </row>
-    <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="23">
         <v>7.11</v>
       </c>

</xml_diff>

<commit_message>
modif des matrices du monde 9
</commit_message>
<xml_diff>
--- a/fizzbuzz.xlsx
+++ b/fizzbuzz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jydel\OneDrive\Desktop\FizzBuzz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84799DE7-6A61-4D04-81F0-CFF047D50A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1F27A1-9DD3-4CC5-BF0F-0F0577A4FE7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{ABC71DB8-80FE-454F-B082-C51C83431DFA}"/>
   </bookViews>
@@ -1680,8 +1680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB2EF8FE-7976-455F-A7A2-652D6E5C5BD6}">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2494,7 +2494,7 @@
         <v>5</v>
       </c>
       <c r="M23" s="15">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="N23" s="15">
         <v>6</v>

</xml_diff>